<commit_message>
Modification du tableau Kanban pour les assignations des taches
</commit_message>
<xml_diff>
--- a/Tableau_mini_projet/Tableau Kanban.xlsx
+++ b/Tableau_mini_projet/Tableau Kanban.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3DVP\GIT\mini_projet_tache\Gestionnaire_de_Taches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3DVP\GIT\mini_projet_tache\Gestionnaire_de_Taches\Tableau_mini_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B4D8C30-A852-4BA8-B5B1-D0116E24F5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8417EAAA-DB01-4A32-BC56-D76B938615E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4776F350-C597-4EE6-84E0-C94527FBAF90}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Column1</t>
   </si>
@@ -92,9 +92,6 @@
     <t xml:space="preserve"> - Initialiser le dépôt GitHub                                         </t>
   </si>
   <si>
-    <t xml:space="preserve"> Alice     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Haute    </t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t xml:space="preserve"> - Créer la structure de base du projet                                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Bob       </t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Implémenter la fonction d'ajout de tâches                           </t>
   </si>
   <si>
@@ -126,9 +120,6 @@
   </si>
   <si>
     <t xml:space="preserve"> - Définir les user stories                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Équipe    </t>
   </si>
   <si>
     <t xml:space="preserve"> - Créer le tableau Kanban initial                                     </t>
@@ -213,6 +204,27 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>Teddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teddy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teddy     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ny       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ny     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teddy&amp;Ny    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Teddy&amp;Ny        </t>
   </si>
 </sst>
 </file>
@@ -646,7 +658,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -679,7 +691,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -722,16 +734,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -768,10 +780,10 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
@@ -782,16 +794,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
@@ -802,16 +814,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
@@ -822,16 +834,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>6</v>
@@ -842,16 +854,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>6</v>
@@ -862,16 +874,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
@@ -882,16 +894,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>

</xml_diff>